<commit_message>
[Lib,Test] Fix credit card insert test
</commit_message>
<xml_diff>
--- a/test/max-credit-card_test.xlsx
+++ b/test/max-credit-card_test.xlsx
@@ -21,14 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lohit Devanagari"/>
-        <family val="2"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="58">
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lohit Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">כל המשתמשים </t>
     </r>
@@ -75,6 +76,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ספרות אחרונות של כרטיס האשראי</t>
     </r>
@@ -119,6 +121,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">שער המרה ממטבע מקור</t>
     </r>
@@ -138,6 +141,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">התחשבנות לש</t>
     </r>
@@ -157,6 +161,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ח</t>
     </r>
@@ -189,6 +194,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">תשלום </t>
     </r>
@@ -208,6 +214,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">מתוך </t>
     </r>
@@ -244,6 +251,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">תשלום </t>
     </r>
@@ -263,6 +271,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">מתוך </t>
     </r>
@@ -329,6 +338,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">חיוב עסקת חו</t>
     </r>
@@ -348,6 +358,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ל בש</t>
     </r>
@@ -367,6 +378,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ח </t>
     </r>
@@ -391,6 +403,12 @@
   </si>
   <si>
     <t xml:space="preserve">GOOGLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dalna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
   </si>
 </sst>
 </file>
@@ -428,6 +446,7 @@
       <color rgb="FF000000"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -472,13 +491,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -504,23 +527,23 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="38.03"/>
   </cols>
   <sheetData>
@@ -786,13 +809,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.87"/>
@@ -802,13 +825,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="38.03"/>
   </cols>
   <sheetData>
@@ -1027,6 +1050,22 @@
       </c>
       <c r="O8" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>